<commit_message>
fix bug #118330  #118329
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR0004.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR0004.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFFCD47-4647-421E-A49F-744EA2F5AB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -62,7 +56,7 @@
     <definedName name="関連表" localSheetId="0">#REF!</definedName>
     <definedName name="電子帳票仕様" localSheetId="0">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -72,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm"/>
@@ -315,11 +309,26 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -327,28 +336,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="標準_年間勤務台帳" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準_年間勤務台帳" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,7 +468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -526,7 +520,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -720,20 +714,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF4F81BD"/>
   </sheetPr>
   <dimension ref="A1:AMJ975"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="8.25" customHeight="1"/>
   <cols>
@@ -751,12 +745,12 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
@@ -853,36 +847,36 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
     </row>
     <row r="6" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -909,8 +903,8 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
@@ -937,8 +931,8 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="12"/>
@@ -965,8 +959,8 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
@@ -993,8 +987,8 @@
       <c r="Z9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
       <c r="E10" s="12"/>
@@ -1021,8 +1015,8 @@
       <c r="Z10" s="13"/>
     </row>
     <row r="11" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
@@ -1049,8 +1043,8 @@
       <c r="Z11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="12"/>
@@ -1077,8 +1071,8 @@
       <c r="Z12" s="13"/>
     </row>
     <row r="13" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
@@ -1105,8 +1099,8 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
       <c r="E14" s="12"/>
@@ -1133,8 +1127,8 @@
       <c r="Z14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -1161,8 +1155,8 @@
       <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
       <c r="E16" s="12"/>
@@ -1189,8 +1183,8 @@
       <c r="Z16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -1217,8 +1211,8 @@
       <c r="Z17" s="9"/>
     </row>
     <row r="18" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="12"/>
@@ -1245,8 +1239,8 @@
       <c r="Z18" s="13"/>
     </row>
     <row r="19" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
@@ -1273,8 +1267,8 @@
       <c r="Z19" s="9"/>
     </row>
     <row r="20" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
       <c r="E20" s="12"/>
@@ -1301,8 +1295,8 @@
       <c r="Z20" s="13"/>
     </row>
     <row r="21" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -1329,8 +1323,8 @@
       <c r="Z21" s="9"/>
     </row>
     <row r="22" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
       <c r="E22" s="12"/>
@@ -1357,8 +1351,8 @@
       <c r="Z22" s="13"/>
     </row>
     <row r="23" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -1385,8 +1379,8 @@
       <c r="Z23" s="9"/>
     </row>
     <row r="24" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="12"/>
@@ -1413,8 +1407,8 @@
       <c r="Z24" s="13"/>
     </row>
     <row r="25" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -1441,8 +1435,8 @@
       <c r="Z25" s="9"/>
     </row>
     <row r="26" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
       <c r="E26" s="12"/>
@@ -1469,8 +1463,8 @@
       <c r="Z26" s="13"/>
     </row>
     <row r="27" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -1497,8 +1491,8 @@
       <c r="Z27" s="9"/>
     </row>
     <row r="28" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
       <c r="E28" s="12"/>
@@ -1525,8 +1519,8 @@
       <c r="Z28" s="13"/>
     </row>
     <row r="29" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
@@ -1553,8 +1547,8 @@
       <c r="Z29" s="9"/>
     </row>
     <row r="30" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="12"/>
@@ -1581,8 +1575,8 @@
       <c r="Z30" s="13"/>
     </row>
     <row r="31" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
@@ -1609,8 +1603,8 @@
       <c r="Z31" s="9"/>
     </row>
     <row r="32" spans="1:26" ht="8.25" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
       <c r="E32" s="12"/>
@@ -1637,8 +1631,8 @@
       <c r="Z32" s="13"/>
     </row>
     <row r="33" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
@@ -1665,8 +1659,8 @@
       <c r="Z33" s="9"/>
     </row>
     <row r="34" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
       <c r="E34" s="12"/>
@@ -1693,8 +1687,8 @@
       <c r="Z34" s="13"/>
     </row>
     <row r="35" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
@@ -1721,8 +1715,8 @@
       <c r="Z35" s="9"/>
     </row>
     <row r="36" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
@@ -1749,8 +1743,8 @@
       <c r="Z36" s="13"/>
     </row>
     <row r="37" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="8"/>
@@ -1805,256 +1799,256 @@
       <c r="Z38" s="18"/>
     </row>
     <row r="39" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
-      <c r="T39" s="22"/>
-      <c r="U39" s="22"/>
-      <c r="V39" s="22"/>
-      <c r="W39" s="22"/>
-      <c r="X39" s="22"/>
-      <c r="Y39" s="22"/>
-      <c r="Z39" s="22"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="25"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
     </row>
     <row r="40" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="24"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="24"/>
+      <c r="Z40" s="24"/>
     </row>
     <row r="41" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="25"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
     </row>
     <row r="42" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28"/>
-      <c r="P42" s="28"/>
-      <c r="Q42" s="28"/>
-      <c r="R42" s="28"/>
-      <c r="S42" s="28"/>
-      <c r="T42" s="28"/>
-      <c r="U42" s="28"/>
-      <c r="V42" s="28"/>
-      <c r="W42" s="28"/>
-      <c r="X42" s="28"/>
-      <c r="Y42" s="28"/>
-      <c r="Z42" s="28"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="24"/>
+      <c r="Z42" s="24"/>
     </row>
     <row r="43" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="25"/>
-      <c r="U43" s="25"/>
-      <c r="V43" s="25"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-      <c r="Y43" s="25"/>
-      <c r="Z43" s="25"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
+      <c r="Z43" s="21"/>
     </row>
     <row r="44" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28"/>
-      <c r="P44" s="28"/>
-      <c r="Q44" s="28"/>
-      <c r="R44" s="28"/>
-      <c r="S44" s="28"/>
-      <c r="T44" s="28"/>
-      <c r="U44" s="28"/>
-      <c r="V44" s="28"/>
-      <c r="W44" s="28"/>
-      <c r="X44" s="28"/>
-      <c r="Y44" s="28"/>
-      <c r="Z44" s="28"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+      <c r="Y44" s="24"/>
+      <c r="Z44" s="24"/>
     </row>
     <row r="45" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="25"/>
-      <c r="U45" s="25"/>
-      <c r="V45" s="25"/>
-      <c r="W45" s="25"/>
-      <c r="X45" s="25"/>
-      <c r="Y45" s="25"/>
-      <c r="Z45" s="25"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="21"/>
     </row>
     <row r="46" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="28"/>
-      <c r="S46" s="28"/>
-      <c r="T46" s="28"/>
-      <c r="U46" s="28"/>
-      <c r="V46" s="28"/>
-      <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
-      <c r="Y46" s="28"/>
-      <c r="Z46" s="28"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="24"/>
+      <c r="Z46" s="24"/>
     </row>
     <row r="47" spans="1:36" ht="8.25" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="25"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="25"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="25"/>
-      <c r="T47" s="25"/>
-      <c r="U47" s="25"/>
-      <c r="V47" s="25"/>
-      <c r="W47" s="25"/>
-      <c r="X47" s="25"/>
-      <c r="Y47" s="25"/>
-      <c r="Z47" s="25"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="21"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="21"/>
+      <c r="Z47" s="21"/>
     </row>
     <row r="48" spans="1:36" ht="8.25" customHeight="1">
       <c r="A48" s="19"/>
@@ -37322,19 +37316,132 @@
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="U47:V47"/>
-    <mergeCell ref="W47:X47"/>
-    <mergeCell ref="Y47:Z47"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="W39:X39"/>
+    <mergeCell ref="Y39:Z39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="W40:X40"/>
+    <mergeCell ref="Y40:Z40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="W41:X41"/>
+    <mergeCell ref="Y41:Z41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="U43:V43"/>
+    <mergeCell ref="W43:X43"/>
+    <mergeCell ref="Y43:Z43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="Y44:Z44"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
     <mergeCell ref="S45:T45"/>
     <mergeCell ref="U45:V45"/>
     <mergeCell ref="W45:X45"/>
@@ -37359,132 +37466,19 @@
     <mergeCell ref="I45:J45"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="M45:N45"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="U43:V43"/>
-    <mergeCell ref="W43:X43"/>
-    <mergeCell ref="Y43:Z43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="Y44:Z44"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="W41:X41"/>
-    <mergeCell ref="Y41:Z41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="W39:X39"/>
-    <mergeCell ref="Y39:Z39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="W40:X40"/>
-    <mergeCell ref="Y40:Z40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="U47:V47"/>
+    <mergeCell ref="W47:X47"/>
+    <mergeCell ref="Y47:Z47"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="Q47:R47"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1" right="1" top="1.5" bottom="1.5" header="0.8" footer="0.8"/>

</xml_diff>